<commit_message>
Learning Python & Building userguide
Starten met het leren van python en gelijktijdig een userguide schrijven
hiervoor
</commit_message>
<xml_diff>
--- a/01 - Python Research/Journal/Python Journal.xlsx
+++ b/01 - Python Research/Journal/Python Journal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Research Python</t>
   </si>
@@ -34,6 +34,27 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Start Uur</t>
+  </si>
+  <si>
+    <t>Stop Uur</t>
+  </si>
+  <si>
+    <t>Opstarten research project</t>
+  </si>
+  <si>
+    <t>Besloten om python research te doen</t>
+  </si>
+  <si>
+    <t>Maken mappenstructuur en GIT</t>
+  </si>
+  <si>
+    <t>Kiezen leermethode/platform: "Codecademy"</t>
+  </si>
+  <si>
+    <t>Afgewerkte Codecademy lessen:</t>
   </si>
 </sst>
 </file>
@@ -93,12 +114,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Linked Cell" xfId="1" builtinId="24"/>
@@ -380,26 +402,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="147.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="156.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:7" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -407,28 +431,93 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>42939</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.61388888888888882</v>
+      </c>
+      <c r="F6" s="5">
+        <f>E6-D6</f>
+        <v>6.4583333333333215E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.71736111111111101</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" ref="F7:F11" si="0">E7-D7</f>
+        <v>4.7916666666666607E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Datetime & Strings and Console Output
</commit_message>
<xml_diff>
--- a/01 - Python Research/Journal/Python Journal.xlsx
+++ b/01 - Python Research/Journal/Python Journal.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Research Python</t>
   </si>
@@ -54,7 +54,16 @@
     <t>Kiezen leermethode/platform: "Codecademy"</t>
   </si>
   <si>
-    <t>Afgewerkte Codecademy lessen:</t>
+    <t>Verderzetten Research</t>
+  </si>
+  <si>
+    <t>Afgewerkte hoofdstukken: "Python Syntax"</t>
+  </si>
+  <si>
+    <t>Afgewerkte hoofdstukken: "Strings and Console Output, Date &amp; Time"</t>
+  </si>
+  <si>
+    <t>Verder instuderen Python en verder ontwikkelen cursus</t>
   </si>
 </sst>
 </file>
@@ -114,13 +123,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Linked Cell" xfId="1" builtinId="24"/>
@@ -472,7 +483,7 @@
         <v>0.71736111111111101</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" ref="F7:F11" si="0">E7-D7</f>
+        <f t="shared" ref="F7:F12" si="0">E7-D7</f>
         <v>4.7916666666666607E-2</v>
       </c>
       <c r="G7" t="s">
@@ -488,24 +499,48 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
       <c r="F9" s="5"/>
       <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>42944</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="5"/>
+      <c r="D12" s="5">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>7.638888888888884E-2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
       <c r="F13" s="5"/>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" s="5"/>
@@ -513,10 +548,10 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28" s="5"/>
     </row>
   </sheetData>

</xml_diff>